<commit_message>
Renombrar CIUDAD AUTONOMA DE BUENOS AIRES a CABA en todos los gráficos de provincias
</commit_message>
<xml_diff>
--- a/lideres_post.xlsx
+++ b/lideres_post.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BB\Downloads\fusion telefonica telecom\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840DA492-7D02-45CA-AFA4-FA7A2D3BC7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$26</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -130,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,14 +188,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -194,13 +217,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -238,7 +269,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -272,6 +303,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -306,9 +338,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,14 +514,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -519,16 +559,16 @@
         <v>1681772.344008341</v>
       </c>
       <c r="D2">
-        <v>0.3261193111907678</v>
+        <v>0.32611931119076781</v>
       </c>
       <c r="E2">
-        <v>2609218.86548627</v>
+        <v>2609218.8654862698</v>
       </c>
       <c r="F2">
-        <v>0.5059642359977581</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.50596423599775808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -536,19 +576,19 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <v>32264.71527969346</v>
+        <v>32264.715279693461</v>
       </c>
       <c r="D3">
-        <v>0.5079163380869667</v>
+        <v>0.50791633808696668</v>
       </c>
       <c r="E3">
-        <v>32264.71527969346</v>
+        <v>32264.715279693461</v>
       </c>
       <c r="F3">
-        <v>0.5079163380869667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.50791633808696668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -556,19 +596,19 @@
         <v>31</v>
       </c>
       <c r="C4">
-        <v>79843.92158832563</v>
+        <v>79843.921588325626</v>
       </c>
       <c r="D4">
         <v>0.4092253688808335</v>
       </c>
       <c r="E4">
-        <v>79843.92158832563</v>
+        <v>79843.921588325626</v>
       </c>
       <c r="F4">
         <v>0.4092253688808335</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -579,16 +619,16 @@
         <v>126.8027836151756</v>
       </c>
       <c r="D5">
-        <v>0.000845052382436608</v>
+        <v>8.4505238243660799E-4</v>
       </c>
       <c r="E5">
-        <v>65519.85581529792</v>
+        <v>65519.855815297917</v>
       </c>
       <c r="F5">
-        <v>0.4366442807884401</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.43664428078844009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -596,19 +636,19 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>565025.7675063371</v>
+        <v>565025.76750633714</v>
       </c>
       <c r="D6">
-        <v>0.4249821772572194</v>
+        <v>0.42498217725721937</v>
       </c>
       <c r="E6">
-        <v>716294.5762833068</v>
+        <v>716294.57628330681</v>
       </c>
       <c r="F6">
-        <v>0.538758488714416</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.53875848871441601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -616,19 +656,19 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>409682.2897286013</v>
+        <v>409682.28972860129</v>
       </c>
       <c r="D7">
-        <v>0.447056992089606</v>
+        <v>0.44705699208960598</v>
       </c>
       <c r="E7">
-        <v>410012.1258025864</v>
+        <v>410012.12580258638</v>
       </c>
       <c r="F7">
-        <v>0.4474169186151488</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0.44741691861514882</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -636,19 +676,19 @@
         <v>31</v>
       </c>
       <c r="C8">
-        <v>88130.76663329748</v>
+        <v>88130.766633297477</v>
       </c>
       <c r="D8">
-        <v>0.4886907603780742</v>
+        <v>0.48869076037807418</v>
       </c>
       <c r="E8">
-        <v>88130.76663329748</v>
+        <v>88130.766633297477</v>
       </c>
       <c r="F8">
-        <v>0.4886907603780742</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0.48869076037807418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -659,36 +699,36 @@
         <v>147680.6244558192</v>
       </c>
       <c r="D9">
-        <v>0.5449078106206137</v>
+        <v>0.54490781062061366</v>
       </c>
       <c r="E9">
-        <v>149820.2799547639</v>
+        <v>149820.27995476389</v>
       </c>
       <c r="F9">
-        <v>0.5528026512451608</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.55280265124516081</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C10">
-        <v>34007.3694577467</v>
+        <v>34007.369457746703</v>
       </c>
       <c r="D10">
-        <v>0.4349050280373</v>
+        <v>0.43490502803730002</v>
       </c>
       <c r="E10">
-        <v>34007.3694577467</v>
+        <v>34007.369457746703</v>
       </c>
       <c r="F10">
-        <v>0.4349050280373</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0.43490502803730002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -696,19 +736,19 @@
         <v>33</v>
       </c>
       <c r="C11">
-        <v>33486.0702578539</v>
+        <v>33486.070257853899</v>
       </c>
       <c r="D11">
-        <v>0.2850755603608544</v>
+        <v>0.28507556036085441</v>
       </c>
       <c r="E11">
-        <v>33486.0702578539</v>
+        <v>33486.070257853899</v>
       </c>
       <c r="F11">
-        <v>0.2850755603608544</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>0.28507556036085441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -716,39 +756,39 @@
         <v>34</v>
       </c>
       <c r="C12">
-        <v>40970.28701005953</v>
+        <v>40970.287010059532</v>
       </c>
       <c r="D12">
-        <v>0.5316039854272256</v>
+        <v>0.53160398542722564</v>
       </c>
       <c r="E12">
-        <v>40970.28701005953</v>
+        <v>40970.287010059532</v>
       </c>
       <c r="F12">
-        <v>0.5316039854272255</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0.53160398542722553</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C13">
-        <v>46930.52441397266</v>
+        <v>46930.524413972656</v>
       </c>
       <c r="D13">
-        <v>0.6275990188791599</v>
+        <v>0.62759901887915992</v>
       </c>
       <c r="E13">
-        <v>46930.52441397266</v>
+        <v>46930.524413972656</v>
       </c>
       <c r="F13">
-        <v>0.6275990188791599</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>0.62759901887915992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -756,19 +796,19 @@
         <v>31</v>
       </c>
       <c r="C14">
-        <v>11605.77646128021</v>
+        <v>11605.776461280209</v>
       </c>
       <c r="D14">
-        <v>0.03911375412422407</v>
+        <v>3.9113754124224069E-2</v>
       </c>
       <c r="E14">
-        <v>111758.8430494523</v>
+        <v>111758.84304945231</v>
       </c>
       <c r="F14">
-        <v>0.3766493282743991</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>0.37664932827439912</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -776,19 +816,19 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>84240.43555024256</v>
+        <v>84240.435550242561</v>
       </c>
       <c r="D15">
-        <v>0.4004475107653357</v>
+        <v>0.40044751076533569</v>
       </c>
       <c r="E15">
-        <v>84240.43555024256</v>
+        <v>84240.435550242561</v>
       </c>
       <c r="F15">
-        <v>0.4004475107653357</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0.40044751076533569</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -796,19 +836,19 @@
         <v>33</v>
       </c>
       <c r="C16">
-        <v>71237.21735643537</v>
+        <v>71237.217356435372</v>
       </c>
       <c r="D16">
-        <v>0.4735687103636291</v>
+        <v>0.47356871036362908</v>
       </c>
       <c r="E16">
-        <v>71237.21735643537</v>
+        <v>71237.217356435372</v>
       </c>
       <c r="F16">
-        <v>0.473568710363629</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>0.47356871036362902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -822,13 +862,13 @@
         <v>0.1863890811682706</v>
       </c>
       <c r="E17">
-        <v>81140.73793939331</v>
+        <v>81140.737939393308</v>
       </c>
       <c r="F17">
-        <v>0.5483015054043235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>0.54830150540432354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -836,19 +876,19 @@
         <v>31</v>
       </c>
       <c r="C18">
-        <v>101052.1867700941</v>
+        <v>101052.18677009409</v>
       </c>
       <c r="D18">
-        <v>0.4435670967072637</v>
+        <v>0.44356709670726369</v>
       </c>
       <c r="E18">
-        <v>101052.1867700941</v>
+        <v>101052.18677009409</v>
       </c>
       <c r="F18">
-        <v>0.4435670967072637</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>0.44356709670726369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -856,19 +896,19 @@
         <v>31</v>
       </c>
       <c r="C19">
-        <v>7171.812336856148</v>
+        <v>7171.8123368561482</v>
       </c>
       <c r="D19">
-        <v>0.05599859539586523</v>
+        <v>5.5998595395865228E-2</v>
       </c>
       <c r="E19">
-        <v>65586.2982402799</v>
+        <v>65586.298240279895</v>
       </c>
       <c r="F19">
-        <v>0.5121077359756979</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>0.51210773597569792</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -876,19 +916,19 @@
         <v>33</v>
       </c>
       <c r="C20">
-        <v>57328.00010094119</v>
+        <v>57328.000100941194</v>
       </c>
       <c r="D20">
         <v>0.5806000685613254</v>
       </c>
       <c r="E20">
-        <v>57328.00010094119</v>
+        <v>57328.000100941194</v>
       </c>
       <c r="F20">
         <v>0.5806000685613254</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -896,19 +936,19 @@
         <v>33</v>
       </c>
       <c r="C21">
-        <v>34864.05644919094</v>
+        <v>34864.056449190939</v>
       </c>
       <c r="D21">
-        <v>0.5737696782265365</v>
+        <v>0.57376967822653646</v>
       </c>
       <c r="E21">
-        <v>34864.05644919094</v>
+        <v>34864.056449190939</v>
       </c>
       <c r="F21">
-        <v>0.5737696782265365</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>0.57376967822653646</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -916,39 +956,39 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>393273.3602697235</v>
+        <v>393273.36026972352</v>
       </c>
       <c r="D22">
-        <v>0.4568510344076439</v>
+        <v>0.45685103440764391</v>
       </c>
       <c r="E22">
-        <v>393273.3602697235</v>
+        <v>393273.36026972352</v>
       </c>
       <c r="F22">
-        <v>0.4568510344076439</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0.45685103440764391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
-        <v>33</v>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C23">
-        <v>56715.46689587441</v>
+        <v>56715.466895874408</v>
       </c>
       <c r="D23">
-        <v>0.4464616148819786</v>
+        <v>0.44646161488197861</v>
       </c>
       <c r="E23">
-        <v>56715.46689587441</v>
+        <v>56715.466895874408</v>
       </c>
       <c r="F23">
-        <v>0.4464616148819786</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>0.44646161488197861</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -956,19 +996,19 @@
         <v>35</v>
       </c>
       <c r="C24">
-        <v>21968.73932694565</v>
+        <v>21968.739326945652</v>
       </c>
       <c r="D24">
-        <v>0.4253815812836427</v>
+        <v>0.42538158128364267</v>
       </c>
       <c r="E24">
-        <v>21968.73932694565</v>
+        <v>21968.739326945652</v>
       </c>
       <c r="F24">
-        <v>0.4253815812836427</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>0.42538158128364267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -979,16 +1019,16 @@
         <v>121128.6038759275</v>
       </c>
       <c r="D25">
-        <v>0.4018407882572796</v>
+        <v>0.40184078825727959</v>
       </c>
       <c r="E25">
         <v>121128.6038759275</v>
       </c>
       <c r="F25">
-        <v>0.4018407882572796</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>0.40184078825727959</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -999,16 +1039,23 @@
         <v>36228.50716651808</v>
       </c>
       <c r="D26">
-        <v>0.120187069043494</v>
+        <v>0.12018706904349399</v>
       </c>
       <c r="E26">
         <v>36228.50716651808</v>
       </c>
       <c r="F26">
-        <v>0.120187069043494</v>
+        <v>0.12018706904349399</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F26" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Flow"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>